<commit_message>
Employee Data Full Logic
</commit_message>
<xml_diff>
--- a/config/table_config copy.xlsx
+++ b/config/table_config copy.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="52">
   <si>
     <t>DOMAIN</t>
   </si>
@@ -126,6 +126,51 @@
   </si>
   <si>
     <t>EQUNR,SPRAS,TEXT_DESCR</t>
+  </si>
+  <si>
+    <t>employee</t>
+  </si>
+  <si>
+    <t>S_EMPLOYEE</t>
+  </si>
+  <si>
+    <t>PERNR</t>
+  </si>
+  <si>
+    <t>S_PA0000</t>
+  </si>
+  <si>
+    <t>PERNR,ENDDA,BEGDA,MASSN,MASSG,STAT2</t>
+  </si>
+  <si>
+    <t>S_PA0001</t>
+  </si>
+  <si>
+    <t>PERNR,ENDDA,BEGDA,BUKRS,WERKS,VDSK1,BTRTL,KOSTL,KOKRS,PERSG,PERSK,ORGEH,OTYPE,MSTBR</t>
+  </si>
+  <si>
+    <t>S_PA0002</t>
+  </si>
+  <si>
+    <t>PERNR,ENDDA,BEGDA,INITS,NACHN,NACH2,VORNA,TITEL,MIDNM,SPRSL</t>
+  </si>
+  <si>
+    <t>S_PA0006</t>
+  </si>
+  <si>
+    <t>SUBTY,ENDDA,BEGDA,ANSSA,STRAS,ORT01,ORT02,PSTLZ,LAND1,LOCAT,ADR03,ADR04,STATE,HSNMR,BLDNG,FLOOR,STRDS,COUNC,RCTVC,COM01,NUM01,COM02,NUM02,COM03,NUM03,COM04,NUM04,COM05,NUM05,COM06,NUM06</t>
+  </si>
+  <si>
+    <t>S_PA0105</t>
+  </si>
+  <si>
+    <t>PERNR,SUBTY,ENDDA,BEGDA,USRTY</t>
+  </si>
+  <si>
+    <t>S_INFOTYPE_TEXT</t>
+  </si>
+  <si>
+    <t>INFTY,SUBTY,ENDDA,BEGDA</t>
   </si>
 </sst>
 </file>
@@ -197,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -212,6 +257,12 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -525,20 +576,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="25.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="26.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="20.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="141.57642857142858" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="25.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="26.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="20.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="141.57642857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -555,7 +606,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -572,7 +623,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -589,7 +640,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -606,7 +657,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -623,7 +674,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -640,7 +691,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -657,7 +708,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -674,7 +725,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
@@ -691,7 +742,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
@@ -708,7 +759,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
@@ -725,7 +776,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -742,7 +793,7 @@
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
@@ -759,7 +810,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="4" t="s">
         <v>29</v>
       </c>
@@ -776,7 +827,7 @@
         <v>32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="4" t="s">
         <v>29</v>
       </c>
@@ -810,12 +861,124 @@
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="5"/>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18">
+      <c r="A17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="6">
+        <v>2</v>
+      </c>
+      <c r="D17" s="6">
+        <v>1</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18">
+      <c r="A18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="6">
+        <v>4</v>
+      </c>
+      <c r="D18" s="6">
+        <v>2</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18">
+      <c r="A19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="6">
+        <v>4</v>
+      </c>
+      <c r="D19" s="6">
+        <v>3</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18">
+      <c r="A20" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="6">
+        <v>4</v>
+      </c>
+      <c r="D20" s="6">
+        <v>4</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18">
+      <c r="A21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="6">
+        <v>4</v>
+      </c>
+      <c r="D21" s="6">
+        <v>4</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18">
+      <c r="A22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="6">
+        <v>4</v>
+      </c>
+      <c r="D22" s="6">
+        <v>5</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+      <c r="A23" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="3">
+        <v>4</v>
+      </c>
+      <c r="D23" s="3">
+        <v>6</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Materials Logic - first changes
</commit_message>
<xml_diff>
--- a/config/table_config copy.xlsx
+++ b/config/table_config copy.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="65">
   <si>
     <t>DOMAIN</t>
   </si>
@@ -171,6 +171,45 @@
   </si>
   <si>
     <t>INFTY,SUBTY,ENDDA,BEGDA</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>S_CUST_GEN</t>
+  </si>
+  <si>
+    <t>S_CUST_SALES_DATA</t>
+  </si>
+  <si>
+    <t>S_CUST_SALES_PARTNER</t>
+  </si>
+  <si>
+    <t>S_CUST_COMPANY</t>
+  </si>
+  <si>
+    <t>S_CUST_BANK_DATA</t>
+  </si>
+  <si>
+    <t>S_CUST_CC_DATA</t>
+  </si>
+  <si>
+    <t>S_CUST_INDUSTRY</t>
+  </si>
+  <si>
+    <t>S_CUST_TAXCLASS</t>
+  </si>
+  <si>
+    <t>S_CUST_TAXNUMBERS</t>
+  </si>
+  <si>
+    <t>S_CUST_IDENT</t>
+  </si>
+  <si>
+    <t>S_CUST_CONT</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -178,7 +217,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,6 +235,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -242,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -259,10 +304,22 @@
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -576,20 +633,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="25.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="26.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="20.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="10" width="141.57642857142858" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="12" width="25.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="12" width="26.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="13" width="20.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="13" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="14" width="141.57642857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -606,7 +663,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -623,7 +680,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -640,7 +697,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -657,7 +714,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -674,7 +731,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -691,7 +748,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -708,7 +765,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -725,7 +782,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
@@ -742,7 +799,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
@@ -759,7 +816,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
@@ -776,7 +833,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -793,7 +850,7 @@
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
@@ -810,7 +867,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="4" t="s">
         <v>29</v>
       </c>
@@ -827,7 +884,7 @@
         <v>32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="4" t="s">
         <v>29</v>
       </c>
@@ -861,7 +918,7 @@
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
       <c r="A17" s="4" t="s">
         <v>37</v>
       </c>
@@ -878,7 +935,7 @@
         <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
       <c r="A18" s="4" t="s">
         <v>37</v>
       </c>
@@ -895,7 +952,7 @@
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
       <c r="A19" s="4" t="s">
         <v>37</v>
       </c>
@@ -912,7 +969,7 @@
         <v>43</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
       <c r="A20" s="4" t="s">
         <v>37</v>
       </c>
@@ -929,7 +986,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
       <c r="A21" s="4" t="s">
         <v>37</v>
       </c>
@@ -946,7 +1003,7 @@
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
       <c r="A22" s="4" t="s">
         <v>37</v>
       </c>
@@ -963,7 +1020,7 @@
         <v>49</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
       <c r="A23" s="4" t="s">
         <v>37</v>
       </c>
@@ -978,6 +1035,217 @@
       </c>
       <c r="E23" s="5" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+      <c r="A24" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="8">
+        <v>20000</v>
+      </c>
+      <c r="D24" s="8">
+        <v>1</v>
+      </c>
+      <c r="E24" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+      <c r="A25" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="8">
+        <v>20000</v>
+      </c>
+      <c r="D25" s="8">
+        <v>2</v>
+      </c>
+      <c r="E25" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+      <c r="A26" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="8">
+        <v>20000</v>
+      </c>
+      <c r="D26" s="8">
+        <v>3</v>
+      </c>
+      <c r="E26" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+      <c r="A27" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="8">
+        <v>20000</v>
+      </c>
+      <c r="D27" s="8">
+        <v>4</v>
+      </c>
+      <c r="E27" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
+      <c r="A28" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="8">
+        <v>20000</v>
+      </c>
+      <c r="D28" s="8">
+        <v>5</v>
+      </c>
+      <c r="E28" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
+      <c r="A29" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="8">
+        <v>20000</v>
+      </c>
+      <c r="D29" s="8">
+        <v>6</v>
+      </c>
+      <c r="E29" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
+      <c r="A30" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="8">
+        <v>20000</v>
+      </c>
+      <c r="D30" s="8">
+        <v>7</v>
+      </c>
+      <c r="E30" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
+      <c r="A31" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="8">
+        <v>20000</v>
+      </c>
+      <c r="D31" s="8">
+        <v>8</v>
+      </c>
+      <c r="E31" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
+      <c r="A32" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="8">
+        <v>20000</v>
+      </c>
+      <c r="D32" s="8">
+        <v>9</v>
+      </c>
+      <c r="E32" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
+      <c r="A33" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="8">
+        <v>20000</v>
+      </c>
+      <c r="D33" s="8">
+        <v>10</v>
+      </c>
+      <c r="E33" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
+      <c r="A34" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="8">
+        <v>20000</v>
+      </c>
+      <c r="D34" s="8">
+        <v>11</v>
+      </c>
+      <c r="E34" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
+      <c r="A35" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
+      <c r="A36" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
+      <c r="A37" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
+      <c r="A38" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="11" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes Done for Employee, Equipment and Vendor
</commit_message>
<xml_diff>
--- a/config/table_config copy.xlsx
+++ b/config/table_config copy.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="80">
   <si>
     <t>DOMAIN</t>
   </si>
@@ -109,10 +109,6 @@
     <t>S_EQUI</t>
   </si>
   <si>
-    <t xml:space="preserve">40,000
-</t>
-  </si>
-  <si>
     <t>EQUNR,NRANGE_IND,EQTYP,DATAB,EQKTX,BRGEW,GEWEI,MATNR,GERNR</t>
   </si>
   <si>
@@ -209,7 +205,55 @@
     <t>S_CUST_CONT</t>
   </si>
   <si>
-    <t/>
+    <t>material</t>
+  </si>
+  <si>
+    <t>S_MARA</t>
+  </si>
+  <si>
+    <t>S_MAKT</t>
+  </si>
+  <si>
+    <t>S_MARM</t>
+  </si>
+  <si>
+    <t>S_MEAN</t>
+  </si>
+  <si>
+    <t>S_MVKE</t>
+  </si>
+  <si>
+    <t>S_MLAN</t>
+  </si>
+  <si>
+    <t>S_MARC</t>
+  </si>
+  <si>
+    <t>S_MARD</t>
+  </si>
+  <si>
+    <t>S_MRP_AREA</t>
+  </si>
+  <si>
+    <t>S_MLGN</t>
+  </si>
+  <si>
+    <t>S_MLGT</t>
+  </si>
+  <si>
+    <t>S_MBEW</t>
+  </si>
+  <si>
+    <t>S_MBEW_CURRENT</t>
+  </si>
+  <si>
+    <t>S_MBEW_FUTURE</t>
+  </si>
+  <si>
+    <t>SAPAPO_MATLSP</t>
+  </si>
+  <si>
+    <t>MARC</t>
   </si>
 </sst>
 </file>
@@ -287,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -314,12 +358,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -633,17 +671,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="12" width="25.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="26.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="20.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="13" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="14" width="141.57642857142858" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="25.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="26.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="20.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="11" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="12" width="141.57642857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -671,7 +709,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="3">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
@@ -688,7 +726,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="3">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D3" s="3">
         <v>2</v>
@@ -705,7 +743,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="3">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D4" s="3">
         <v>3</v>
@@ -722,7 +760,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="3">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
@@ -739,7 +777,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="3">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D6" s="3">
         <v>5</v>
@@ -756,7 +794,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="3">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D7" s="3">
         <v>6</v>
@@ -773,7 +811,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="3">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D8" s="3">
         <v>7</v>
@@ -790,7 +828,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="3">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D9" s="3">
         <v>8</v>
@@ -807,7 +845,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="3">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D10" s="3">
         <v>9</v>
@@ -824,7 +862,7 @@
         <v>24</v>
       </c>
       <c r="C11" s="3">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D11" s="3">
         <v>10</v>
@@ -841,7 +879,7 @@
         <v>25</v>
       </c>
       <c r="C12" s="3">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D12" s="3">
         <v>11</v>
@@ -858,7 +896,7 @@
         <v>27</v>
       </c>
       <c r="C13" s="3">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D13" s="3">
         <v>12</v>
@@ -874,14 +912,14 @@
       <c r="B14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="3">
+        <v>20000</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="D14" s="3">
-        <v>12</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
@@ -889,16 +927,16 @@
         <v>29</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="3">
+        <v>20000</v>
+      </c>
+      <c r="D15" s="3">
+        <v>2</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="C15" s="3">
-        <v>40000</v>
-      </c>
-      <c r="D15" s="3">
-        <v>13</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
@@ -906,126 +944,126 @@
         <v>29</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="3">
+        <v>20000</v>
+      </c>
+      <c r="D16" s="3">
+        <v>3</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="C16" s="3">
-        <v>40000</v>
-      </c>
-      <c r="D16" s="3">
-        <v>14</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
       <c r="A17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="C17" s="3">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="C17" s="6">
-        <v>2</v>
-      </c>
-      <c r="D17" s="6">
-        <v>1</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
       <c r="A18" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="3">
+        <v>4</v>
+      </c>
+      <c r="D18" s="3">
+        <v>2</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="C18" s="6">
-        <v>4</v>
-      </c>
-      <c r="D18" s="6">
-        <v>2</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>41</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
       <c r="A19" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="3">
+        <v>4</v>
+      </c>
+      <c r="D19" s="3">
+        <v>3</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="6">
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+      <c r="A20" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="3">
         <v>4</v>
       </c>
-      <c r="D19" s="6">
-        <v>3</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
-      <c r="A20" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="4" t="s">
+      <c r="D20" s="3">
+        <v>4</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="6">
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+      <c r="A21" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="3">
         <v>4</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D21" s="3">
         <v>4</v>
       </c>
-      <c r="E20" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
-      <c r="A21" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="4" t="s">
+      <c r="E21" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="6">
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+      <c r="A22" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="3">
         <v>4</v>
       </c>
-      <c r="D21" s="6">
-        <v>4</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
-      <c r="A22" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="4" t="s">
+      <c r="D22" s="3">
+        <v>5</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="6">
-        <v>4</v>
-      </c>
-      <c r="D22" s="6">
-        <v>5</v>
-      </c>
-      <c r="E22" s="7" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+      <c r="A23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
-      <c r="A23" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="C23" s="3">
         <v>4</v>
@@ -1034,219 +1072,381 @@
         <v>6</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
       <c r="A24" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="8">
-        <v>20000</v>
-      </c>
-      <c r="D24" s="8">
+      <c r="C24" s="6">
+        <v>20000</v>
+      </c>
+      <c r="D24" s="6">
         <v>1</v>
       </c>
-      <c r="E24" s="9"/>
+      <c r="E24" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
       <c r="A25" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="8">
-        <v>20000</v>
-      </c>
-      <c r="D25" s="8">
+        <v>53</v>
+      </c>
+      <c r="C25" s="6">
+        <v>20000</v>
+      </c>
+      <c r="D25" s="6">
         <v>2</v>
       </c>
-      <c r="E25" s="9"/>
+      <c r="E25" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
       <c r="A26" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="8">
-        <v>20000</v>
-      </c>
-      <c r="D26" s="8">
+        <v>54</v>
+      </c>
+      <c r="C26" s="6">
+        <v>20000</v>
+      </c>
+      <c r="D26" s="6">
         <v>3</v>
       </c>
-      <c r="E26" s="9"/>
+      <c r="E26" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
       <c r="A27" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="8">
-        <v>20000</v>
-      </c>
-      <c r="D27" s="8">
+        <v>55</v>
+      </c>
+      <c r="C27" s="6">
+        <v>20000</v>
+      </c>
+      <c r="D27" s="6">
         <v>4</v>
       </c>
-      <c r="E27" s="9"/>
+      <c r="E27" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
       <c r="A28" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="8">
-        <v>20000</v>
-      </c>
-      <c r="D28" s="8">
+        <v>56</v>
+      </c>
+      <c r="C28" s="6">
+        <v>20000</v>
+      </c>
+      <c r="D28" s="6">
         <v>5</v>
       </c>
-      <c r="E28" s="9"/>
+      <c r="E28" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
       <c r="A29" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="8">
-        <v>20000</v>
-      </c>
-      <c r="D29" s="8">
+        <v>57</v>
+      </c>
+      <c r="C29" s="6">
+        <v>20000</v>
+      </c>
+      <c r="D29" s="6">
         <v>6</v>
       </c>
-      <c r="E29" s="9"/>
+      <c r="E29" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
       <c r="A30" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="8">
-        <v>20000</v>
-      </c>
-      <c r="D30" s="8">
+        <v>58</v>
+      </c>
+      <c r="C30" s="6">
+        <v>20000</v>
+      </c>
+      <c r="D30" s="6">
         <v>7</v>
       </c>
-      <c r="E30" s="9"/>
+      <c r="E30" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
       <c r="A31" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" s="8">
-        <v>20000</v>
-      </c>
-      <c r="D31" s="8">
+        <v>59</v>
+      </c>
+      <c r="C31" s="6">
+        <v>20000</v>
+      </c>
+      <c r="D31" s="6">
         <v>8</v>
       </c>
-      <c r="E31" s="9"/>
+      <c r="E31" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
       <c r="A32" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="8">
-        <v>20000</v>
-      </c>
-      <c r="D32" s="8">
+        <v>60</v>
+      </c>
+      <c r="C32" s="6">
+        <v>20000</v>
+      </c>
+      <c r="D32" s="6">
         <v>9</v>
       </c>
-      <c r="E32" s="9"/>
+      <c r="E32" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
       <c r="A33" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C33" s="8">
-        <v>20000</v>
-      </c>
-      <c r="D33" s="8">
+        <v>61</v>
+      </c>
+      <c r="C33" s="6">
+        <v>20000</v>
+      </c>
+      <c r="D33" s="6">
         <v>10</v>
       </c>
-      <c r="E33" s="9"/>
+      <c r="E33" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
       <c r="A34" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C34" s="8">
-        <v>20000</v>
-      </c>
-      <c r="D34" s="8">
+        <v>62</v>
+      </c>
+      <c r="C34" s="6">
+        <v>20000</v>
+      </c>
+      <c r="D34" s="6">
         <v>11</v>
       </c>
-      <c r="E34" s="9"/>
+      <c r="E34" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B35" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="9"/>
+      <c r="C35" s="6">
+        <v>20000</v>
+      </c>
+      <c r="D35" s="6"/>
+      <c r="E35" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
-      <c r="A36" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="9"/>
+      <c r="A36" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" s="6">
+        <v>20000</v>
+      </c>
+      <c r="D36" s="6"/>
+      <c r="E36" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
-      <c r="A37" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
-      <c r="A38" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="11" t="s">
-        <v>64</v>
-      </c>
+      <c r="A37" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="6">
+        <v>20000</v>
+      </c>
+      <c r="D37" s="6"/>
+      <c r="E37" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18">
+      <c r="A38" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="8">
+        <v>20000</v>
+      </c>
+      <c r="D38" s="8"/>
+      <c r="E38" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18">
+      <c r="A39" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" s="8">
+        <v>20000</v>
+      </c>
+      <c r="D39" s="8"/>
+      <c r="E39" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18">
+      <c r="A40" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" s="8">
+        <v>20000</v>
+      </c>
+      <c r="D40" s="8"/>
+      <c r="E40" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18">
+      <c r="A41" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="8">
+        <v>20000</v>
+      </c>
+      <c r="D41" s="8"/>
+      <c r="E41" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18">
+      <c r="A42" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" s="8">
+        <v>20000</v>
+      </c>
+      <c r="D42" s="8"/>
+      <c r="E42" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18">
+      <c r="A43" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" s="8">
+        <v>20000</v>
+      </c>
+      <c r="D43" s="8"/>
+      <c r="E43" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18">
+      <c r="A44" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C44" s="8">
+        <v>20000</v>
+      </c>
+      <c r="D44" s="8"/>
+      <c r="E44" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18">
+      <c r="A45" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C45" s="8">
+        <v>20000</v>
+      </c>
+      <c r="D45" s="8"/>
+      <c r="E45" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18">
+      <c r="A46" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C46" s="8">
+        <v>20000</v>
+      </c>
+      <c r="D46" s="8"/>
+      <c r="E46" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18">
+      <c r="A47" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C47" s="8">
+        <v>20000</v>
+      </c>
+      <c r="D47" s="8"/>
+      <c r="E47" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18">
+      <c r="A48" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C48" s="8">
+        <v>20000</v>
+      </c>
+      <c r="D48" s="8"/>
+      <c r="E48" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18">
+      <c r="A49" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C49" s="8">
+        <v>20000</v>
+      </c>
+      <c r="D49" s="8"/>
+      <c r="E49" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18">
+      <c r="A50" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C50" s="8">
+        <v>20000</v>
+      </c>
+      <c r="D50" s="8"/>
+      <c r="E50" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>